<commit_message>
Adds project progress tracking files
Adds a markdown file and several excel files to track project progress.

The markdown file seems to contain information for a meeting on July 15, 2025.
The excel file contains data for tracking project progress from January to June 2025.
</commit_message>
<xml_diff>
--- a/인천보고서_202501.xlsx
+++ b/인천보고서_202501.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\IdeaProjects\sidogeumgo\src\md\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\sidogeumgo_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97810C3C-59BF-4653-8E46-55C5A09A197D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50794FF-8C70-428E-9230-8AFFEDACE2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="상세내역" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">상세내역!$A$4:$J$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">상세내역!$A$1:$H$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">상세내역!$A$4:$J$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">상세내역!$A$1:$H$49</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
   <si>
     <t>품질관리 상세근거</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -77,14 +77,6 @@
     <t>긴급요청
 여부</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>지적여부</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>비 고</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>개발 및
@@ -472,13 +464,55 @@
     <t>보고서 개선을 위한 신규 집계 적용</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>시간</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>문의: 2
+업무확인: 3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무확인:4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무확인:24</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무확인:16</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무확인:48</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발:12
+산출물:4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발:6건 12시간
+업무확인:11건 151시간
+산출물:1건 4시간
+문의:2건 2시간</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -1067,7 +1101,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1084,9 +1118,6 @@
     <xf numFmtId="58" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1262,6 +1293,84 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1274,21 +1383,6 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1298,62 +1392,47 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1669,62 +1748,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B28" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" style="18" customWidth="1"/>
-    <col min="2" max="2" width="82.625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="10.25" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.75" style="23" customWidth="1"/>
-    <col min="5" max="5" width="98.625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="9.75" style="23" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="23.625" style="23" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="18"/>
+    <col min="1" max="1" width="14" style="17" customWidth="1"/>
+    <col min="2" max="2" width="82.625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="10.25" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" style="22" customWidth="1"/>
+    <col min="5" max="5" width="98.625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="9.75" style="110" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="23.625" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="82" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
+      <c r="A2" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="86" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
@@ -1742,975 +1821,1004 @@
       <c r="E4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="98" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="391.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="391.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="87" t="s">
+      <c r="C5" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="D5" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="E5" s="81"/>
+      <c r="F5" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="91" t="s">
+      <c r="G5" s="83" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="67"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="77"/>
+      <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="92"/>
-      <c r="F5" s="94" t="s">
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="68"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="77"/>
+      <c r="B7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="94" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="78"/>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="88"/>
-      <c r="B6" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="79"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="88"/>
-      <c r="B7" s="11" t="s">
+      <c r="E7" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="65">
+        <v>4</v>
+      </c>
+      <c r="G7" s="65">
+        <v>5</v>
+      </c>
+      <c r="H7" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="119.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="77"/>
+      <c r="B8" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="52"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="77"/>
+      <c r="B9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="65">
+        <v>1</v>
+      </c>
+      <c r="G9" s="65">
+        <v>4</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="77"/>
+      <c r="B10" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="52"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="77"/>
+      <c r="B11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="65">
+        <v>7</v>
+      </c>
+      <c r="G11" s="65">
+        <v>16</v>
+      </c>
+      <c r="H11" s="66" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="324" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="77"/>
+      <c r="B12" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="52"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="77"/>
+      <c r="B13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="52"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="77"/>
+      <c r="B14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="65">
+        <v>1</v>
+      </c>
+      <c r="G14" s="65">
+        <v>16</v>
+      </c>
+      <c r="H14" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="77"/>
+      <c r="B15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="52"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="77"/>
+      <c r="B16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="65">
+        <v>3</v>
+      </c>
+      <c r="G16" s="65">
+        <v>24</v>
+      </c>
+      <c r="H16" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="77"/>
+      <c r="B17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="52"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="77"/>
+      <c r="B18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="52"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="77"/>
+      <c r="B19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="52"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="77"/>
+      <c r="B20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="65">
+        <v>1</v>
+      </c>
+      <c r="G20" s="65">
+        <v>24</v>
+      </c>
+      <c r="H20" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="77"/>
+      <c r="B21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="52"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="77"/>
+      <c r="B22" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C22" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="65">
+        <v>1</v>
+      </c>
+      <c r="G22" s="65">
+        <v>16</v>
+      </c>
+      <c r="H22" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="77"/>
+      <c r="B23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="52"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="77"/>
+      <c r="B24" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="E24" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="52"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="77"/>
+      <c r="B25" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="52"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="77"/>
+      <c r="B26" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="53"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="119.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="88"/>
-      <c r="B8" s="11" t="s">
+      <c r="E26" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="65">
+        <v>1</v>
+      </c>
+      <c r="G26" s="65">
+        <v>16</v>
+      </c>
+      <c r="H26" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="77"/>
+      <c r="B27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="52"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="77"/>
+      <c r="B28" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="52"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="77"/>
+      <c r="B29" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="53"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="88"/>
-      <c r="B9" s="11" t="s">
+      <c r="C29" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="65">
+        <v>1</v>
+      </c>
+      <c r="G29" s="65">
+        <v>48</v>
+      </c>
+      <c r="H29" s="52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="1" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="77"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="65">
+        <f>SUM(F7:F29)</f>
+        <v>20</v>
+      </c>
+      <c r="G30" s="65">
+        <f>SUM(G7:G29)</f>
+        <v>169</v>
+      </c>
+      <c r="H30" s="111" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="77"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="111"/>
+    </row>
+    <row r="32" spans="1:10" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="53"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="29"/>
+    </row>
+    <row r="33" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="53"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="102"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="29"/>
+    </row>
+    <row r="34" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="53"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="102"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="29"/>
+    </row>
+    <row r="35" spans="1:8" s="63" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="57"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="62"/>
+    </row>
+    <row r="36" spans="1:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="88" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="87" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="88" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" s="104" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="24"/>
+    </row>
+    <row r="37" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="69"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="104"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="24"/>
+    </row>
+    <row r="38" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="69"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="85"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="14"/>
+    </row>
+    <row r="39" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="69"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="14"/>
+    </row>
+    <row r="40" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="69"/>
+      <c r="B40" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="53"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="88"/>
-      <c r="B10" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="53"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="88"/>
-      <c r="B11" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="53"/>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="324" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="88"/>
-      <c r="B12" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="53"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="88"/>
-      <c r="B13" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C13" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="53"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="88"/>
-      <c r="B14" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="53"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="88"/>
-      <c r="B15" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="53"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="88"/>
-      <c r="B16" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="53"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="88"/>
-      <c r="B17" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="53"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="88"/>
-      <c r="B18" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="53"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="88"/>
-      <c r="B19" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="11" t="s">
+      <c r="D40" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="14"/>
+    </row>
+    <row r="41" spans="1:8" s="1" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="69"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="102"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="33"/>
+    </row>
+    <row r="42" spans="1:8" s="41" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="84" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="53"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="88"/>
-      <c r="B20" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="53"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="88"/>
-      <c r="B21" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="53"/>
-      <c r="J21" s="9"/>
-    </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="88"/>
-      <c r="B22" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="53"/>
-      <c r="J22" s="9"/>
-    </row>
-    <row r="23" spans="1:10" s="1" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="88"/>
-      <c r="B23" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="53"/>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="88"/>
-      <c r="B24" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="53"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="1:10" s="1" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="88"/>
-      <c r="B25" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="53"/>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="88"/>
-      <c r="B26" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="53"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="88"/>
-      <c r="B27" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="53"/>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="1:10" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="88"/>
-      <c r="B28" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="53"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="1:10" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="88"/>
-      <c r="B29" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="53"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="1:10" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="88"/>
-      <c r="B30" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="53"/>
-    </row>
-    <row r="31" spans="1:10" s="1" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="88"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="53"/>
-    </row>
-    <row r="32" spans="1:10" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="88"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="53"/>
-    </row>
-    <row r="33" spans="1:8" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="54"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="30"/>
-    </row>
-    <row r="34" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="54"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="30"/>
-    </row>
-    <row r="35" spans="1:8" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="54"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="30"/>
-    </row>
-    <row r="36" spans="1:8" s="64" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="58"/>
-      <c r="B36" s="59"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="63"/>
-    </row>
-    <row r="37" spans="1:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="96" t="s">
+      <c r="E42" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="72" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="95" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" s="96" t="s">
-        <v>80</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" s="25"/>
-    </row>
-    <row r="38" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="80"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="25"/>
-    </row>
-    <row r="39" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="80"/>
-      <c r="B39" s="70"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" s="15"/>
-    </row>
-    <row r="40" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="80"/>
-      <c r="B40" s="71"/>
-      <c r="C40" s="74"/>
-      <c r="D40" s="74"/>
-      <c r="E40" s="71"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="15"/>
-    </row>
-    <row r="41" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="80"/>
-      <c r="B41" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H41" s="15"/>
-    </row>
-    <row r="42" spans="1:8" s="1" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="80"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="34"/>
-    </row>
-    <row r="43" spans="1:8" s="42" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="66" t="s">
+      <c r="F42" s="105" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="40"/>
+    </row>
+    <row r="43" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="92"/>
+      <c r="B43" s="89"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="96"/>
+      <c r="F43" s="104"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="24"/>
+    </row>
+    <row r="44" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="92"/>
+      <c r="B44" s="89"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="85"/>
+      <c r="E44" s="96"/>
+      <c r="F44" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="14"/>
+    </row>
+    <row r="45" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="92"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="97"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="14"/>
+    </row>
+    <row r="46" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="92"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="14"/>
+    </row>
+    <row r="47" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="92"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="14"/>
+    </row>
+    <row r="48" spans="1:8" s="26" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="93"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="106"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="44"/>
+    </row>
+    <row r="49" spans="1:8" s="1" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="69" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="72" t="s">
+      <c r="B49" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43" s="75" t="s">
-        <v>82</v>
-      </c>
-      <c r="F43" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G43" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="41"/>
-    </row>
-    <row r="44" spans="1:8" s="1" customFormat="1" ht="235.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="67"/>
-      <c r="B44" s="70"/>
-      <c r="C44" s="73"/>
-      <c r="D44" s="73"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="25"/>
-    </row>
-    <row r="45" spans="1:8" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="67"/>
-      <c r="B45" s="70"/>
-      <c r="C45" s="73"/>
-      <c r="D45" s="73"/>
-      <c r="E45" s="76"/>
-      <c r="F45" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G45" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H45" s="15"/>
-    </row>
-    <row r="46" spans="1:8" s="1" customFormat="1" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="67"/>
-      <c r="B46" s="71"/>
-      <c r="C46" s="74"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="77"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="15"/>
-    </row>
-    <row r="47" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="67"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H47" s="15"/>
-    </row>
-    <row r="48" spans="1:8" s="1" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="67"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="15"/>
-    </row>
-    <row r="49" spans="1:8" s="27" customFormat="1" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="68"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="45"/>
-    </row>
-    <row r="50" spans="1:8" s="1" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="35" t="s">
+      <c r="C49" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" s="36" t="s">
+      <c r="E49" s="30"/>
+      <c r="F49" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="G50" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="H50" s="39"/>
-    </row>
-    <row r="51" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+      <c r="G49" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="38"/>
+    </row>
+    <row r="50" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="F50" s="108"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="109"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="20"/>
+    </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="109"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="20"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="21"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="109"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="20"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="21"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="109"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="20"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="21"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="109"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="20"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="21"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="109"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="20"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="21"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="109"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="20"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="21"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="109"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="20"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="21"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="109"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="20"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="21"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="109"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="20"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B61" s="1"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="21"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="109"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="20"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="21"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="109"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="20"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="21"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="109"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="20"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="21"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="21"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="22"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="21"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="1"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="22"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="21"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="22"/>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B68" s="1"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="22"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="E42:E45"/>
     <mergeCell ref="H5:H6"/>
-    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A36:A41"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A5:A32"/>
+    <mergeCell ref="A5:A31"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A43:A49"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="D43:D46"/>
-    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="B36:B39"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.3" right="0" top="0.3" bottom="0.11811023622047245" header="0.22" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="28" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="49" max="7" man="1"/>
+    <brk id="48" max="7" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>